<commit_message>
test data run flag marked to yes
</commit_message>
<xml_diff>
--- a/test-suite/ecommerce/src/main/resources/testdata/testdata.xlsx
+++ b/test-suite/ecommerce/src/main/resources/testdata/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N.Kumar8\eclipse-workspace\test-suite\ecommerce\src\main\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N.Kumar8\git\Maven\test-suite\ecommerce\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A7ECAF-6E51-4F9B-BF79-76A3EB9A9ED1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E247CBAA-9A38-4D10-ACC2-C8A539C8260E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
     <t>verify_aom_edit_order</t>
   </si>
   <si>
-    <t>no</t>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1418,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
test data run flag change
</commit_message>
<xml_diff>
--- a/test-suite/ecommerce/src/main/resources/testdata/testdata.xlsx
+++ b/test-suite/ecommerce/src/main/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N.Kumar8\git\Maven\test-suite\ecommerce\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E247CBAA-9A38-4D10-ACC2-C8A539C8260E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECA2C02-1E69-4A11-BA69-5C70A140B061}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
   <si>
     <t>sl_no</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1421,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B9"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" customHeight="1"/>
@@ -1965,7 +1968,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="4" t="s">
@@ -1992,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="4" t="s">
@@ -2019,7 +2022,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="4" t="s">

</xml_diff>

<commit_message>
dynamic suitexmlfile change in maven pom.xml
</commit_message>
<xml_diff>
--- a/test-suite/ecommerce/src/main/resources/testdata/testdata.xlsx
+++ b/test-suite/ecommerce/src/main/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N.Kumar8\git\Maven\test-suite\ecommerce\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECA2C02-1E69-4A11-BA69-5C70A140B061}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC33C97D-E226-4475-A317-E27266EAD654}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,7 +1421,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" customHeight="1"/>
@@ -1860,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="4" t="s">
@@ -1887,7 +1887,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="4" t="s">
@@ -1914,7 +1914,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="4" t="s">
@@ -1941,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="4" t="s">

</xml_diff>